<commit_message>
Add read and write scripts
</commit_message>
<xml_diff>
--- a/other_xlsx/v0.keep.xlsx
+++ b/other_xlsx/v0.keep.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nxn\Documents\GitHub\python4accountants\other_xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b1510899a56a4b7d/Documents/GitHub/python4accountants/other_xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CB0485-B425-4EDD-A37F-544EE07E2371}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{42CB0485-B425-4EDD-A37F-544EE07E2371}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F614EA41-2782-464D-8179-95523A4B73FE}"/>
   <bookViews>
     <workbookView xWindow="384" yWindow="252" windowWidth="17280" windowHeight="8964" xr2:uid="{6750D065-E144-421E-B181-BDED2FC1B447}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>text</t>
   </si>
@@ -35,9 +35,6 @@
     <t>date</t>
   </si>
   <si>
-    <t>boolan</t>
-  </si>
-  <si>
     <t>datetime</t>
   </si>
   <si>
@@ -141,6 +138,39 @@
   </si>
   <si>
     <t>fruit</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Lisbon</t>
+  </si>
+  <si>
+    <t>Shanghai</t>
+  </si>
+  <si>
+    <t>Tokyo</t>
+  </si>
+  <si>
+    <t>Camberra</t>
+  </si>
+  <si>
+    <t>boolean</t>
   </si>
 </sst>
 </file>
@@ -518,114 +548,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D3CD27-FA09-4EAE-A0FA-EA5B1DD4B2ED}">
-  <dimension ref="B2:D11"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" t="str">
+      <c r="B2" t="str">
         <f>"this is some text"</f>
         <v>this is some text</v>
       </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="str">
+      <c r="B3" t="str">
         <f>"=""this is also some text"""</f>
         <v>="this is also some text"</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="B5">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <v>44197</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3">
+        <v>44197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
         <v>10</v>
-      </c>
-      <c r="C6">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2">
-        <v>44197</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3">
-        <v>44197</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1">
-        <v>44197</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -636,10 +666,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70CFA655-6BA8-4DD3-977B-CCA8E971A778}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -649,103 +679,157 @@
     <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>64</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>85</v>
+      </c>
+      <c r="E7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
         <v>26</v>
       </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>55</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="C9" t="s">
-        <v>29</v>
+      <c r="D9">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -769,13 +853,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -783,7 +867,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -794,7 +878,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -805,7 +889,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -816,7 +900,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -827,7 +911,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6">
         <v>6</v>
@@ -838,7 +922,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -849,7 +933,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -860,7 +944,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -871,7 +955,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10">
         <v>8</v>
@@ -882,7 +966,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C11">
         <v>5</v>

</xml_diff>

<commit_message>
Add first exploration and manipulation of df
</commit_message>
<xml_diff>
--- a/other_xlsx/v0.keep.xlsx
+++ b/other_xlsx/v0.keep.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b1510899a56a4b7d/Documents/GitHub/python4accountants/other_xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{42CB0485-B425-4EDD-A37F-544EE07E2371}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F614EA41-2782-464D-8179-95523A4B73FE}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{42CB0485-B425-4EDD-A37F-544EE07E2371}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B1CB890F-CB68-45F5-BD9A-75DA1C9ACF33}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="252" windowWidth="17280" windowHeight="8964" xr2:uid="{6750D065-E144-421E-B181-BDED2FC1B447}"/>
+    <workbookView xWindow="384" yWindow="252" windowWidth="14028" windowHeight="7476" activeTab="3" xr2:uid="{6750D065-E144-421E-B181-BDED2FC1B447}"/>
   </bookViews>
   <sheets>
     <sheet name="data_types" sheetId="1" r:id="rId1"/>
     <sheet name="people" sheetId="2" r:id="rId2"/>
-    <sheet name="expenses" sheetId="3" r:id="rId3"/>
+    <sheet name="managers" sheetId="4" r:id="rId3"/>
+    <sheet name="expenses" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
   <si>
     <t>text</t>
   </si>
@@ -171,6 +172,42 @@
   </si>
   <si>
     <t>boolean</t>
+  </si>
+  <si>
+    <t>carol</t>
+  </si>
+  <si>
+    <t>brian</t>
+  </si>
+  <si>
+    <t>stephanie</t>
+  </si>
+  <si>
+    <t>dylan</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>bravo</t>
+  </si>
+  <si>
+    <t>charlie</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>Copenhagen</t>
+  </si>
+  <si>
+    <t>Alger</t>
+  </si>
+  <si>
+    <t>Cairo</t>
+  </si>
+  <si>
+    <t>Lima</t>
   </si>
 </sst>
 </file>
@@ -550,7 +587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D3CD27-FA09-4EAE-A0FA-EA5B1DD4B2ED}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -838,11 +875,116 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC6398A4-8E5B-4A8B-92C5-265F33E7FA83}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3">
+        <v>64</v>
+      </c>
+      <c r="E3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{377D020A-AD83-45E3-A181-0C0057CC5C5C}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -963,7 +1105,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>8</v>
+        <v>102</v>
       </c>
       <c r="B11" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Add filter and add_col scripts
</commit_message>
<xml_diff>
--- a/other_xlsx/v0.keep.xlsx
+++ b/other_xlsx/v0.keep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b1510899a56a4b7d/Documents/GitHub/python4accountants/other_xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="13_ncr:1_{42CB0485-B425-4EDD-A37F-544EE07E2371}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B1CB890F-CB68-45F5-BD9A-75DA1C9ACF33}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{42CB0485-B425-4EDD-A37F-544EE07E2371}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7937A78C-23D0-4831-B325-5166A94619E4}"/>
   <bookViews>
     <workbookView xWindow="384" yWindow="252" windowWidth="14028" windowHeight="7476" activeTab="3" xr2:uid="{6750D065-E144-421E-B181-BDED2FC1B447}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
   <si>
     <t>text</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>Lima</t>
+  </si>
+  <si>
+    <t>qty</t>
   </si>
 </sst>
 </file>
@@ -981,10 +984,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{377D020A-AD83-45E3-A181-0C0057CC5C5C}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -993,7 +996,7 @@
     <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -1003,8 +1006,11 @@
       <c r="C1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1012,10 +1018,13 @@
         <v>30</v>
       </c>
       <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1023,10 +1032,13 @@
         <v>32</v>
       </c>
       <c r="C3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1034,10 +1046,13 @@
         <v>31</v>
       </c>
       <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1045,10 +1060,13 @@
         <v>30</v>
       </c>
       <c r="C5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1056,10 +1074,13 @@
         <v>32</v>
       </c>
       <c r="C6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1067,10 +1088,13 @@
         <v>33</v>
       </c>
       <c r="C7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1078,10 +1102,13 @@
         <v>34</v>
       </c>
       <c r="C8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1089,10 +1116,13 @@
         <v>30</v>
       </c>
       <c r="C9">
+        <v>26</v>
+      </c>
+      <c r="D9">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1100,10 +1130,13 @@
         <v>31</v>
       </c>
       <c r="C10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>102</v>
       </c>
@@ -1111,6 +1144,219 @@
         <v>35</v>
       </c>
       <c r="C11">
+        <v>47</v>
+      </c>
+      <c r="D11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12">
+        <v>29</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14">
+        <v>76</v>
+      </c>
+      <c r="D14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>18</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>7</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16">
+        <v>90</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17">
+        <v>25</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18">
+        <v>62</v>
+      </c>
+      <c r="D18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19">
+        <v>95</v>
+      </c>
+      <c r="D19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20">
+        <v>96</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21">
+        <v>99</v>
+      </c>
+      <c r="D21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22">
+        <v>69</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23">
+        <v>81</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>102</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24">
+        <v>12</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25">
+        <v>18</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>103</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26">
+        <v>35</v>
+      </c>
+      <c r="D26">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve scripts with additional examples
</commit_message>
<xml_diff>
--- a/other_xlsx/v0.keep.xlsx
+++ b/other_xlsx/v0.keep.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b1510899a56a4b7d/Documents/GitHub/python4accountants/other_xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{42CB0485-B425-4EDD-A37F-544EE07E2371}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7937A78C-23D0-4831-B325-5166A94619E4}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{42CB0485-B425-4EDD-A37F-544EE07E2371}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5D74A167-29F5-4B3A-BAD2-32B3F066C8E5}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="252" windowWidth="14028" windowHeight="7476" activeTab="3" xr2:uid="{6750D065-E144-421E-B181-BDED2FC1B447}"/>
+    <workbookView xWindow="384" yWindow="252" windowWidth="15768" windowHeight="9120" activeTab="1" xr2:uid="{6750D065-E144-421E-B181-BDED2FC1B447}"/>
   </bookViews>
   <sheets>
     <sheet name="data_types" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="60">
   <si>
     <t>text</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>gold</t>
-  </si>
-  <si>
-    <t>mat</t>
   </si>
   <si>
     <t>master</t>
@@ -689,7 +686,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -708,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70CFA655-6BA8-4DD3-977B-CCA8E971A778}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -730,10 +727,10 @@
         <v>14</v>
       </c>
       <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
         <v>37</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -750,7 +747,7 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -767,7 +764,7 @@
         <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -784,7 +781,7 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -801,24 +798,21 @@
         <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
       </c>
       <c r="D6">
         <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -826,16 +820,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
         <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
       </c>
       <c r="D7">
         <v>85</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -843,16 +837,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
         <v>25</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
       </c>
       <c r="D8">
         <v>55</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -860,16 +854,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
         <v>27</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
       </c>
       <c r="D9">
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -903,10 +897,10 @@
         <v>14</v>
       </c>
       <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
         <v>37</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -914,16 +908,16 @@
         <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2">
         <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -931,16 +925,16 @@
         <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3">
         <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -948,16 +942,16 @@
         <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4">
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -965,16 +959,16 @@
         <v>103</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5">
         <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -986,7 +980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{377D020A-AD83-45E3-A181-0C0057CC5C5C}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -1001,13 +995,13 @@
         <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1015,7 +1009,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2">
         <v>65</v>
@@ -1029,7 +1023,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3">
         <v>71</v>
@@ -1043,7 +1037,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4">
         <v>14</v>
@@ -1057,7 +1051,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>71</v>
@@ -1071,7 +1065,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6">
         <v>33</v>
@@ -1085,7 +1079,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7">
         <v>97</v>
@@ -1099,7 +1093,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1113,7 +1107,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9">
         <v>26</v>
@@ -1127,7 +1121,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -1141,7 +1135,7 @@
         <v>102</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11">
         <v>47</v>
@@ -1155,7 +1149,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12">
         <v>29</v>
@@ -1169,7 +1163,7 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13">
         <v>6</v>
@@ -1183,7 +1177,7 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14">
         <v>76</v>
@@ -1197,7 +1191,7 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15">
         <v>18</v>
@@ -1211,7 +1205,7 @@
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16">
         <v>90</v>
@@ -1225,7 +1219,7 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17">
         <v>25</v>
@@ -1239,7 +1233,7 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18">
         <v>62</v>
@@ -1253,7 +1247,7 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19">
         <v>95</v>
@@ -1267,7 +1261,7 @@
         <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20">
         <v>96</v>
@@ -1281,7 +1275,7 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21">
         <v>99</v>
@@ -1295,7 +1289,7 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22">
         <v>69</v>
@@ -1309,7 +1303,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23">
         <v>81</v>
@@ -1323,7 +1317,7 @@
         <v>102</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C24">
         <v>12</v>
@@ -1337,7 +1331,7 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C25">
         <v>18</v>
@@ -1351,7 +1345,7 @@
         <v>103</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26">
         <v>35</v>

</xml_diff>